<commit_message>
metaPro workflow v2 rolled out.
</commit_message>
<xml_diff>
--- a/storage/mappings/EMSL48473_JGI1781_Stegen_DatasetToMetagenomeMapping_2021-01-25.xlsx
+++ b/storage/mappings/EMSL48473_JGI1781_Stegen_DatasetToMetagenomeMapping_2021-01-25.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pnl\Projects\NMDC_proposal\Anubhav\storage\test\mappings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anub229/Downloads/metaPro/storage/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1CFECE-02AC-0F49-BBA7-CA045DEDD28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="675" windowWidth="28800" windowHeight="16245"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCMS2 match to NMDC metaGs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -103,7 +104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -471,33 +472,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" customWidth="1"/>
     <col min="13" max="13" width="83" customWidth="1"/>
-    <col min="14" max="14" width="30.42578125" customWidth="1"/>
-    <col min="15" max="15" width="86.28515625" customWidth="1"/>
+    <col min="14" max="14" width="30.5" customWidth="1"/>
+    <col min="15" max="15" width="86.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +545,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>500088</v>
       </c>
@@ -594,7 +595,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L34">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L34">
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>